<commit_message>
Final release of V1.0.0
</commit_message>
<xml_diff>
--- a/Production Design Projects/mbedXdotShield/v1.0.0/BOM-Europe.xlsx
+++ b/Production Design Projects/mbedXdotShield/v1.0.0/BOM-Europe.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="MBEDxDOT.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:andcor02:Documents:Eagle:mbed-HDK:mbed-HDK:Production Design Projects:mbedXdotShield:v1.0.0:MBEDxDOT.csv" comma="1" semicolon="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andcor02:Documents:Eagle:mbed-HDK:mbed-HDK:Production Design Projects:mbedXdotShield:v1.0.0:MBEDxDOT.csv" comma="1" semicolon="1">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="211">
   <si>
     <t>Qty</t>
   </si>
@@ -461,9 +461,6 @@
     <t>581-060316C104K</t>
   </si>
   <si>
-    <t>R6, R28</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
@@ -660,6 +657,27 @@
   </si>
   <si>
     <t>1568-1413-ND</t>
+  </si>
+  <si>
+    <t>R6, R27, R28</t>
+  </si>
+  <si>
+    <t>JS202011JCQN</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SLIDE TOGGLE SWITCH VERTICAL (DPDT)</t>
+  </si>
+  <si>
+    <t>C&amp;K Components</t>
+  </si>
+  <si>
+    <t>CKN10723CT-ND</t>
+  </si>
+  <si>
+    <t>611-JS202011JCQN</t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1154,27 +1172,27 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" t="s">
         <v>175</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>176</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>177</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>178</v>
-      </c>
-      <c r="K2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1186,7 +1204,7 @@
         <v>402</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1265,13 +1283,13 @@
         <v>134</v>
       </c>
       <c r="H5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" t="s">
         <v>188</v>
-      </c>
-      <c r="I5" t="s">
-        <v>190</v>
-      </c>
-      <c r="J5" t="s">
-        <v>189</v>
       </c>
       <c r="K5">
         <v>1327666</v>
@@ -1332,19 +1350,19 @@
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" t="s">
         <v>183</v>
-      </c>
-      <c r="K7" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1370,13 +1388,13 @@
         <v>130</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="K8" s="1">
         <v>1458902</v>
@@ -1399,22 +1417,22 @@
         <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" t="s">
         <v>169</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>170</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>171</v>
-      </c>
-      <c r="K9" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1437,16 +1455,16 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" t="s">
         <v>157</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>158</v>
-      </c>
-      <c r="K10" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1469,16 +1487,16 @@
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="K11">
         <v>1514687</v>
@@ -1504,19 +1522,19 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" t="s">
         <v>161</v>
       </c>
-      <c r="H12" t="s">
-        <v>160</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>162</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>163</v>
-      </c>
-      <c r="K12" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1539,19 +1557,19 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H13" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" t="s">
         <v>165</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>166</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>167</v>
-      </c>
-      <c r="K13" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1610,16 +1628,16 @@
         <v>134</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1642,16 +1660,16 @@
         <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="K16" s="1">
         <v>2611902</v>
@@ -1677,16 +1695,16 @@
         <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="K17" s="1">
         <v>2470460</v>
@@ -1712,19 +1730,19 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1814,19 +1832,19 @@
         <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G21" t="s">
         <v>75</v>
       </c>
       <c r="H21" t="s">
+        <v>191</v>
+      </c>
+      <c r="I21" t="s">
         <v>192</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>193</v>
-      </c>
-      <c r="J21" t="s">
-        <v>194</v>
       </c>
       <c r="K21">
         <v>2322069</v>
@@ -1884,19 +1902,19 @@
         <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G23" t="s">
         <v>75</v>
       </c>
       <c r="H23" t="s">
+        <v>195</v>
+      </c>
+      <c r="I23" t="s">
         <v>196</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>197</v>
-      </c>
-      <c r="J23" t="s">
-        <v>198</v>
       </c>
       <c r="K23">
         <v>2322070</v>
@@ -1922,10 +1940,10 @@
         <v>92</v>
       </c>
       <c r="G24" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" t="s">
         <v>203</v>
-      </c>
-      <c r="H24" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2000,7 +2018,7 @@
         <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F27" t="s">
         <v>74</v>
@@ -2099,19 +2117,19 @@
         <v>118</v>
       </c>
       <c r="F30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G30" t="s">
         <v>75</v>
       </c>
       <c r="H30" t="s">
+        <v>198</v>
+      </c>
+      <c r="I30" t="s">
         <v>199</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>200</v>
-      </c>
-      <c r="J30" t="s">
-        <v>201</v>
       </c>
       <c r="K30">
         <v>2322084</v>
@@ -2150,6 +2168,38 @@
       </c>
       <c r="K31">
         <v>2455145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" t="s">
+        <v>208</v>
+      </c>
+      <c r="H32" t="s">
+        <v>205</v>
+      </c>
+      <c r="I32" t="s">
+        <v>209</v>
+      </c>
+      <c r="J32" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change part to D6 to BAT60J
</commit_message>
<xml_diff>
--- a/Production Design Projects/mbedXdotShield/v1.0.0/BOM-Europe.xlsx
+++ b/Production Design Projects/mbedXdotShield/v1.0.0/BOM-Europe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="218">
   <si>
     <t>Qty</t>
   </si>
@@ -236,9 +236,6 @@
     <t>SOD323</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6</t>
-  </si>
-  <si>
     <t>SCHOTTKY DIODE</t>
   </si>
   <si>
@@ -678,6 +675,30 @@
   </si>
   <si>
     <t>611-JS202011JCQN</t>
+  </si>
+  <si>
+    <t>BAT60J</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>BAT60JFILM</t>
+  </si>
+  <si>
+    <t>497-3707-6-ND</t>
+  </si>
+  <si>
+    <t>511-BAT60JFILM</t>
+  </si>
+  <si>
+    <t>89K1218</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5</t>
   </si>
 </sst>
 </file>
@@ -737,8 +758,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -757,19 +782,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1103,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1172,22 +1201,22 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" t="s">
         <v>174</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>175</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>176</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>177</v>
-      </c>
-      <c r="K2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1204,25 +1233,25 @@
         <v>402</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1245,16 +1274,16 @@
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="K4" s="1">
         <v>2302656</v>
@@ -1280,16 +1309,16 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" t="s">
         <v>187</v>
-      </c>
-      <c r="I5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J5" t="s">
-        <v>188</v>
       </c>
       <c r="K5">
         <v>1327666</v>
@@ -1315,16 +1344,16 @@
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="K6" s="1">
         <v>1327679</v>
@@ -1350,19 +1379,19 @@
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" t="s">
         <v>182</v>
-      </c>
-      <c r="K7" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1385,16 +1414,16 @@
         <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="K8" s="1">
         <v>1458902</v>
@@ -1417,22 +1446,22 @@
         <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" t="s">
         <v>168</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>169</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>170</v>
-      </c>
-      <c r="K9" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1455,16 +1484,16 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" t="s">
         <v>156</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>157</v>
-      </c>
-      <c r="K10" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1487,16 +1516,16 @@
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="K11">
         <v>1514687</v>
@@ -1522,19 +1551,19 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" t="s">
         <v>160</v>
       </c>
-      <c r="H12" t="s">
-        <v>159</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>161</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>162</v>
-      </c>
-      <c r="K12" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1557,19 +1586,19 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H13" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" t="s">
         <v>164</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>165</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>166</v>
-      </c>
-      <c r="K13" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1625,19 +1654,19 @@
         <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1660,16 +1689,16 @@
         <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="K16" s="1">
         <v>2611902</v>
@@ -1695,16 +1724,16 @@
         <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="K17" s="1">
         <v>2470460</v>
@@ -1730,19 +1759,19 @@
         <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1782,7 +1811,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
@@ -1794,25 +1823,25 @@
         <v>62</v>
       </c>
       <c r="E20" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>64</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>65</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>66</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>67</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>68</v>
-      </c>
-      <c r="K20" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1820,34 +1849,34 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>210</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="F21" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>212</v>
       </c>
       <c r="H21" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="I21" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="J21" t="s">
-        <v>193</v>
-      </c>
-      <c r="K21">
-        <v>2322069</v>
+        <v>215</v>
+      </c>
+      <c r="K21" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1855,34 +1884,34 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>190</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="J22" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22" t="s">
-        <v>86</v>
+        <v>192</v>
+      </c>
+      <c r="K22">
+        <v>2322069</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1890,34 +1919,34 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
-        <v>194</v>
+        <v>81</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H23" t="s">
-        <v>195</v>
+        <v>78</v>
       </c>
       <c r="I23" t="s">
-        <v>196</v>
+        <v>83</v>
       </c>
       <c r="J23" t="s">
-        <v>197</v>
-      </c>
-      <c r="K23">
-        <v>2322070</v>
+        <v>84</v>
+      </c>
+      <c r="K23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1925,25 +1954,34 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="G24" t="s">
-        <v>202</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>203</v>
+        <v>194</v>
+      </c>
+      <c r="I24" t="s">
+        <v>195</v>
+      </c>
+      <c r="J24" t="s">
+        <v>196</v>
+      </c>
+      <c r="K24">
+        <v>2322070</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1951,28 +1989,25 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="H25" t="s">
-        <v>93</v>
-      </c>
-      <c r="I25" t="s">
-        <v>97</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1980,28 +2015,28 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H26" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I26" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2009,34 +2044,28 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E27" t="s">
-        <v>201</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="I27" t="s">
-        <v>77</v>
-      </c>
-      <c r="J27" t="s">
-        <v>78</v>
-      </c>
-      <c r="K27">
-        <v>2322071</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2044,95 +2073,95 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>200</v>
       </c>
       <c r="F28" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="G28" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="H28" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="I28" t="s">
-        <v>109</v>
-      </c>
-      <c r="K28" t="s">
-        <v>110</v>
+        <v>76</v>
+      </c>
+      <c r="J28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28">
+        <v>2322071</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H29" t="s">
-        <v>111</v>
-      </c>
-      <c r="J29" t="s">
-        <v>115</v>
+        <v>104</v>
+      </c>
+      <c r="I29" t="s">
+        <v>108</v>
+      </c>
+      <c r="K29" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="H30" t="s">
-        <v>198</v>
-      </c>
-      <c r="I30" t="s">
-        <v>199</v>
+        <v>110</v>
       </c>
       <c r="J30" t="s">
-        <v>200</v>
-      </c>
-      <c r="K30">
-        <v>2322084</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2140,34 +2169,34 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E31" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F31" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="G31" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="H31" t="s">
-        <v>119</v>
+        <v>197</v>
       </c>
       <c r="I31" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="J31" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="K31">
-        <v>2455145</v>
+        <v>2322084</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2175,31 +2204,66 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" t="s">
+        <v>122</v>
+      </c>
+      <c r="H32" t="s">
+        <v>118</v>
+      </c>
+      <c r="I32" t="s">
+        <v>123</v>
+      </c>
+      <c r="J32" t="s">
+        <v>124</v>
+      </c>
+      <c r="K32">
+        <v>2455145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" t="s">
         <v>205</v>
       </c>
-      <c r="C32" t="s">
-        <v>205</v>
-      </c>
-      <c r="D32" t="s">
-        <v>205</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F33" t="s">
         <v>206</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G33" t="s">
         <v>207</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H33" t="s">
+        <v>204</v>
+      </c>
+      <c r="I33" t="s">
         <v>208</v>
       </c>
-      <c r="H32" t="s">
-        <v>205</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="J33" t="s">
         <v>209</v>
-      </c>
-      <c r="J32" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>